<commit_message>
Updated code issue in outcome difference tables, started report
</commit_message>
<xml_diff>
--- a/Project1/Reports/DifferenceOutcomesTable09272017_formatted.xlsx
+++ b/Project1/Reports/DifferenceOutcomesTable09272017_formatted.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Total</t>
   </si>
@@ -33,37 +33,49 @@
     <t>Difference in log10 viral load</t>
   </si>
   <si>
-    <t>0.41 ± 0.36</t>
+    <t>0.41 ± 0.37</t>
   </si>
   <si>
     <t>0.39 ± 0.25</t>
   </si>
   <si>
-    <t>0.41 ± 0.37</t>
+    <t>0.41 ± 0.38</t>
   </si>
   <si>
     <t>Difference in CD4+ count</t>
   </si>
   <si>
-    <t>169.3 ± 183.54</t>
+    <t>169.21 ± 183.2</t>
   </si>
   <si>
     <t>13.43 ± 195.73</t>
   </si>
   <si>
-    <t>182.87 ± 176.26</t>
-  </si>
-  <si>
-    <t>2.21 ± 11.99</t>
-  </si>
-  <si>
-    <t>-1.64 ± 8.45</t>
+    <t>183.11 ± 175.67</t>
   </si>
   <si>
     <t>Difference in SF36 MCS score</t>
   </si>
   <si>
+    <t>2.34 ± 12.1</t>
+  </si>
+  <si>
+    <t>3.58 ± 15.07</t>
+  </si>
+  <si>
+    <t>2.23 ± 11.82</t>
+  </si>
+  <si>
     <t>Difference in SF36 PCS score</t>
+  </si>
+  <si>
+    <t>-1.55 ± 8.37</t>
+  </si>
+  <si>
+    <t>-3.85 ± 8.71</t>
+  </si>
+  <si>
+    <t>-1.34 ± 8.32</t>
   </si>
 </sst>
 </file>
@@ -619,22 +631,29 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -643,26 +662,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -987,83 +986,83 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>11</v>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>12</v>
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>